<commit_message>
Atualização dicionario para novo modelo
</commit_message>
<xml_diff>
--- a/Dicionário de dados/Ficha_tecnica.xlsx
+++ b/Dicionário de dados/Ficha_tecnica.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno Girardi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\supor\OneDrive\Área de Trabalho\TrabalhoBD\Dicionário de dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD6F2DA-CF55-46A7-BB5A-A1A8CA4E7915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A4C0CA-89CE-40BF-BF70-A3DF86350D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3DCF4CC4-BC92-4B37-A395-878087F32D44}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3DCF4CC4-BC92-4B37-A395-878087F32D44}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="43">
   <si>
     <t>Tabela</t>
   </si>
@@ -83,18 +83,12 @@
     <t>X</t>
   </si>
   <si>
-    <t>id_produto</t>
-  </si>
-  <si>
     <t>INT</t>
   </si>
   <si>
     <t>1 - sem limite</t>
   </si>
   <si>
-    <t>Referencia o id do produto</t>
-  </si>
-  <si>
     <t>nome</t>
   </si>
   <si>
@@ -107,15 +101,6 @@
     <t>Sabores de bolos disponiveis. 1- Tradicional / 2- Chocolate</t>
   </si>
   <si>
-    <t>sabor_recheio</t>
-  </si>
-  <si>
-    <t>decoracao_bolo</t>
-  </si>
-  <si>
-    <t>sabor_bolo</t>
-  </si>
-  <si>
     <t>Tabela responsável por armazenar dados completos dos bolos</t>
   </si>
   <si>
@@ -128,93 +113,12 @@
     <t>TEXT</t>
   </si>
   <si>
-    <t>manteiga_gramas</t>
-  </si>
-  <si>
-    <t>trigo_gramas</t>
-  </si>
-  <si>
-    <t>Quantidade em gramas de manteiga utilizadas para produção do bolo</t>
-  </si>
-  <si>
-    <t>Quantidade em gramas de trigo utilizadas para produção do bolo</t>
-  </si>
-  <si>
-    <t>acucar_gramas</t>
-  </si>
-  <si>
-    <t>Quantidade em gramas de acucar utilizadas para produção do bolo</t>
-  </si>
-  <si>
-    <t>ovos_unidades</t>
-  </si>
-  <si>
-    <t>Quantidade de unidades de ovos utilizadas para produção do bolo</t>
-  </si>
-  <si>
-    <t>leite_ml</t>
-  </si>
-  <si>
-    <t>Quantidade em MLs de leite utilizadas para produção do bolo</t>
-  </si>
-  <si>
-    <t>fermento_po_gramas</t>
-  </si>
-  <si>
-    <t>Quantidade em gramas de fermento utilizadas para produção do bolo</t>
-  </si>
-  <si>
-    <t>baunilha_ml</t>
-  </si>
-  <si>
-    <t>Quantidade em Mls de baunilha utilizadas para produção do bolo</t>
-  </si>
-  <si>
-    <t>sal_gramas</t>
-  </si>
-  <si>
-    <t>Quantidade em gramas de sal utilizadas para produção do bolo</t>
-  </si>
-  <si>
-    <t>cobertura_gramas</t>
-  </si>
-  <si>
-    <t>Quantidade em gramas de cobertura utilizadas para produção do bolo</t>
-  </si>
-  <si>
-    <t>recheio_gramas</t>
-  </si>
-  <si>
-    <t>Quantidade em gramas de recheio utilizadas para produção do bolo</t>
-  </si>
-  <si>
-    <t>Sabores de bolos para produção. 1- Tradicional / 2- Chocolate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sabores de recheio do bolo para produção.  1- Brigadeiro / 2- Brigadeiro Branco / 3- Dois Amores / 4-Ninho com nutella / 5- Quatro Leites / 6- Sensação / 5- Cocada / 6- Caramelo Salgado </t>
-  </si>
-  <si>
-    <t>Decoração utilizada para produção do bolo. 1- Bento (frase personalizada) / 2- Desenho animado / 3- Time de futebol / 4- Cor lisa, 5- Mandar referencia</t>
-  </si>
-  <si>
-    <t>tempo_producao</t>
-  </si>
-  <si>
     <t>INTERVAL</t>
   </si>
   <si>
     <t>Tempo total para produção do bolo</t>
   </si>
   <si>
-    <t>modo_preparo</t>
-  </si>
-  <si>
-    <t>Descrição total do preparo para o bolo</t>
-  </si>
-  <si>
-    <t>custo_unitario</t>
-  </si>
-  <si>
     <t>DECIMAL</t>
   </si>
   <si>
@@ -225,6 +129,42 @@
   </si>
   <si>
     <t>( 10 , 2 )</t>
+  </si>
+  <si>
+    <t>id_massa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Codigo identificador referenciador do tipo de massa .1- Tradicional / 2- Chocolate </t>
+  </si>
+  <si>
+    <t>id_recheio</t>
+  </si>
+  <si>
+    <t>Codigo identificador referenciador do tipo de massa .1- Bento (frase personalizada) / 2- Desenho animado / 3- Time de futebol / 4- Cor lisa, 5- Mandar referencia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Codigo identificador referenciador do tipo de massa .1- Brigadeiro / 2- Brigadeiro Branco / 3- Dois Amores / 4-Ninho com nutella / 5- Quatro Leites / 6- Sensação / 5- Cocada / 6- Caramelo Salgado </t>
+  </si>
+  <si>
+    <t>id_decoracao</t>
+  </si>
+  <si>
+    <t>tempo_preparo</t>
+  </si>
+  <si>
+    <t>custo_total</t>
+  </si>
+  <si>
+    <t>servicos_utilizados</t>
+  </si>
+  <si>
+    <t>VARCHAR(50)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10 - 50</t>
+  </si>
+  <si>
+    <t>Serviços utilizados para o preparo do bolo</t>
   </si>
 </sst>
 </file>
@@ -277,7 +217,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -300,11 +240,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -313,13 +290,31 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -656,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C77C5C6D-C09F-45C3-B8E6-3C69CA2C291B}">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,44 +676,44 @@
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+        <v>21</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="10"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="6"/>
+      <c r="B4" s="7"/>
       <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
@@ -742,7 +737,7 @@
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="4"/>
+      <c r="B5" s="5"/>
       <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
@@ -757,41 +752,39 @@
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="4"/>
+        <v>17</v>
+      </c>
+      <c r="B6" s="5"/>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F6" s="2"/>
-      <c r="G6" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="4"/>
+      <c r="B7" s="5"/>
       <c r="C7" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>61</v>
+        <v>16</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>13</v>
@@ -799,60 +792,65 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="M7" s="3"/>
+    </row>
+    <row r="8" spans="1:13" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="4"/>
+        <v>31</v>
+      </c>
+      <c r="B8" s="5"/>
       <c r="C8" s="2" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="G8" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="H8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M8" s="3"/>
-    </row>
-    <row r="9" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="4"/>
+        <v>33</v>
+      </c>
+      <c r="B9" s="5"/>
       <c r="C9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+      <c r="G9" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="H9" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="4"/>
+        <v>36</v>
+      </c>
+      <c r="B10" s="5"/>
       <c r="C10" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>13</v>
@@ -860,19 +858,19 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" s="4"/>
+        <v>37</v>
+      </c>
+      <c r="B11" s="5"/>
       <c r="C11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>13</v>
@@ -880,19 +878,19 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="4"/>
+        <v>39</v>
+      </c>
+      <c r="B12" s="5"/>
       <c r="C12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>17</v>
+        <v>40</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>41</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>13</v>
@@ -900,19 +898,19 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="4"/>
+      <c r="B13" s="5"/>
       <c r="C13" s="2" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>13</v>
@@ -920,245 +918,15 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="90" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="M20" s="3"/>
-    </row>
-    <row r="21" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2" t="s">
-        <v>60</v>
-      </c>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N17" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="A24:B24"/>
+  <mergeCells count="13">
     <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A12:B12"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="A3:H3"/>
@@ -1169,6 +937,7 @@
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A12:B12"/>
     <mergeCell ref="A11:B11"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>